<commit_message>
Working on dijkstra implementation
</commit_message>
<xml_diff>
--- a/HourRegistration.xlsx
+++ b/HourRegistration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\GitHub\Repositories\PersonalPortfolio_Q4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33083EBC-6668-427D-9971-D1D0F2D0FA84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87057FD6-3528-44D7-B9C7-229E17A3E303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -74,6 +74,18 @@
   </si>
   <si>
     <t>9.15 - 13.15</t>
+  </si>
+  <si>
+    <t>14.45 - 16.45</t>
+  </si>
+  <si>
+    <t>Continue researching algorithms. Implement cell neighbour finding</t>
+  </si>
+  <si>
+    <t>11.30 - 15.00</t>
+  </si>
+  <si>
+    <t>Implementing dijkstra algorithm</t>
   </si>
 </sst>
 </file>
@@ -395,7 +407,7 @@
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,13 +488,41 @@
         <v>10</v>
       </c>
     </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>44957</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>44958</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>11</v>
       </c>
       <c r="D32">
         <f>SUM(D3:D31)</f>
-        <v>8.25</v>
+        <v>12.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on AI agents
</commit_message>
<xml_diff>
--- a/HourRegistration.xlsx
+++ b/HourRegistration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\GitHub\Repositories\PersonalPortfolio_Q4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87057FD6-3528-44D7-B9C7-229E17A3E303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91A6DD6-0385-43D5-9D77-7E0D9FDC5B91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4680" yWindow="4680" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -86,6 +86,24 @@
   </si>
   <si>
     <t>Implementing dijkstra algorithm</t>
+  </si>
+  <si>
+    <t>10.30 - 13.00</t>
+  </si>
+  <si>
+    <t>9.30 - 14.30</t>
+  </si>
+  <si>
+    <t>Implemented cost field, heatmap</t>
+  </si>
+  <si>
+    <t>10.00 - 12.30</t>
+  </si>
+  <si>
+    <t>9.00 - 12.30</t>
+  </si>
+  <si>
+    <t>Implemented flow field, working on AI agents</t>
   </si>
 </sst>
 </file>
@@ -407,7 +425,7 @@
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,13 +534,66 @@
         <v>16</v>
       </c>
     </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>44959</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8">
+        <v>2.5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>44965</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <v>2.5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>44966</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10">
+        <v>3.5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>44967</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
+    </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>11</v>
       </c>
       <c r="D32">
         <f>SUM(D3:D31)</f>
-        <v>12.25</v>
+        <v>25.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on AI agent behaviour. Refactoring code
</commit_message>
<xml_diff>
--- a/HourRegistration.xlsx
+++ b/HourRegistration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\GitHub\Repositories\PersonalPortfolio_Q4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91A6DD6-0385-43D5-9D77-7E0D9FDC5B91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B34CD3-2646-4F6A-A772-91D44949E817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="4680" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -91,9 +91,6 @@
     <t>10.30 - 13.00</t>
   </si>
   <si>
-    <t>9.30 - 14.30</t>
-  </si>
-  <si>
     <t>Implemented cost field, heatmap</t>
   </si>
   <si>
@@ -104,6 +101,24 @@
   </si>
   <si>
     <t>Implemented flow field, working on AI agents</t>
+  </si>
+  <si>
+    <t>13.30 - 16.00</t>
+  </si>
+  <si>
+    <t>Working on AI agents</t>
+  </si>
+  <si>
+    <t>Implemented basic AI navigation.</t>
+  </si>
+  <si>
+    <t>9.30 - 12.30</t>
+  </si>
+  <si>
+    <t>15.00 - 17.00</t>
+  </si>
+  <si>
+    <t>Researching flocking/boids</t>
   </si>
 </sst>
 </file>
@@ -425,7 +440,7 @@
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="AF33" sqref="AF33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,13 +568,13 @@
         <v>44965</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9">
         <v>2.5</v>
       </c>
       <c r="E9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -567,24 +582,55 @@
         <v>44966</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10">
         <v>3.5</v>
       </c>
       <c r="E10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
+        <v>44966</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11">
+        <v>2.5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>44967</v>
       </c>
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11">
-        <v>5</v>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>44967</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
@@ -593,7 +639,7 @@
       </c>
       <c r="D32">
         <f>SUM(D3:D31)</f>
-        <v>25.75</v>
+        <v>28.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implementing cohesion, avoidance, alignment.
</commit_message>
<xml_diff>
--- a/HourRegistration.xlsx
+++ b/HourRegistration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\GitHub\Repositories\PersonalPortfolio_Q4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B34CD3-2646-4F6A-A772-91D44949E817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4029ADC1-5F21-4D11-8CBA-E5F1804619F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="-15" windowWidth="16440" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -119,6 +119,24 @@
   </si>
   <si>
     <t>Researching flocking/boids</t>
+  </si>
+  <si>
+    <t>Working on flocking/boids</t>
+  </si>
+  <si>
+    <t>13.15 - 15.00</t>
+  </si>
+  <si>
+    <t>11.30-13.30</t>
+  </si>
+  <si>
+    <t>Implemented avoidance, working on alignment</t>
+  </si>
+  <si>
+    <t>Working on alignment &amp; cohesion</t>
+  </si>
+  <si>
+    <t>18.30 - 21.00</t>
   </si>
 </sst>
 </file>
@@ -440,7 +458,7 @@
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AF33" sqref="AF33"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,13 +651,83 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>45047</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14">
+        <v>2.5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>45048</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15">
+        <v>1.75</v>
+      </c>
+      <c r="E15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>45049</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16">
+        <v>1.75</v>
+      </c>
+      <c r="E16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>45051</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>45056</v>
+      </c>
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18">
+        <v>2.5</v>
+      </c>
+      <c r="E18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>11</v>
       </c>
       <c r="D32">
         <f>SUM(D3:D31)</f>
-        <v>28.25</v>
+        <v>38.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reimplemented flocking. Improved neighbour indicators
</commit_message>
<xml_diff>
--- a/HourRegistration.xlsx
+++ b/HourRegistration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\GitHub\Repositories\PersonalPortfolio_Q4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CD41B65-49DC-4C18-9C78-8AFA72BCCF32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C94C1C3F-C9A4-47DD-AE2B-6C560B4CD080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-15" windowWidth="16440" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
   <si>
     <t>Date</t>
   </si>
@@ -143,6 +143,30 @@
   </si>
   <si>
     <t>19.30 - 22.30</t>
+  </si>
+  <si>
+    <t>Reworking flocking</t>
+  </si>
+  <si>
+    <t>18.00 - 22.00</t>
+  </si>
+  <si>
+    <t>July 12th deadline</t>
+  </si>
+  <si>
+    <t>11.00 - 15.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total hours both goals = </t>
+  </si>
+  <si>
+    <t>Total hours=</t>
+  </si>
+  <si>
+    <t>21.00 - 22.15</t>
+  </si>
+  <si>
+    <t>Reimplemented flocking. Improved neighbour finding indicators.</t>
   </si>
 </sst>
 </file>
@@ -461,15 +485,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q32"/>
+  <dimension ref="A1:R37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -477,7 +501,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -496,14 +520,14 @@
       <c r="O2" t="s">
         <v>3</v>
       </c>
-      <c r="P2" t="s">
-        <v>4</v>
-      </c>
       <c r="Q2" t="s">
+        <v>4</v>
+      </c>
+      <c r="R2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44915</v>
       </c>
@@ -516,8 +540,17 @@
       <c r="E3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N3" s="1">
+        <v>45091</v>
+      </c>
+      <c r="O3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44951</v>
       </c>
@@ -530,8 +563,17 @@
       <c r="E4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N4" s="1">
+        <v>45098</v>
+      </c>
+      <c r="O4" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44956</v>
       </c>
@@ -544,8 +586,17 @@
       <c r="E5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N5" s="1">
+        <v>45102</v>
+      </c>
+      <c r="O5" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44957</v>
       </c>
@@ -558,8 +609,17 @@
       <c r="E6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N6" s="1">
+        <v>45105</v>
+      </c>
+      <c r="O6" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44958</v>
       </c>
@@ -572,8 +632,17 @@
       <c r="E7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N7" s="1">
+        <v>45112</v>
+      </c>
+      <c r="O7" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44959</v>
       </c>
@@ -587,7 +656,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44965</v>
       </c>
@@ -601,7 +670,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44966</v>
       </c>
@@ -615,7 +684,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44966</v>
       </c>
@@ -629,7 +698,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44967</v>
       </c>
@@ -643,7 +712,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44967</v>
       </c>
@@ -657,7 +726,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>45047</v>
       </c>
@@ -671,7 +740,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>45048</v>
       </c>
@@ -685,7 +754,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>45049</v>
       </c>
@@ -699,7 +768,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>45051</v>
       </c>
@@ -713,7 +782,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>45056</v>
       </c>
@@ -727,7 +796,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>45062</v>
       </c>
@@ -741,7 +810,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>45063</v>
       </c>
@@ -751,14 +820,110 @@
       <c r="D20">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+      <c r="E20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>45069</v>
+      </c>
+      <c r="B21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>45070</v>
+      </c>
+      <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22">
+        <v>4</v>
+      </c>
+      <c r="E22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>45074</v>
+      </c>
+      <c r="B23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>45077</v>
+      </c>
+      <c r="B24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>45081</v>
+      </c>
+      <c r="B25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>45084</v>
+      </c>
+      <c r="B26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O32" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q32">
+        <f>SUM(Q3:Q31)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>11</v>
       </c>
-      <c r="D32">
-        <f>SUM(D3:D31)</f>
-        <v>43</v>
+      <c r="D33">
+        <f>SUM(D3:D32)</f>
+        <v>64.150000000000006</v>
+      </c>
+    </row>
+    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="J37" t="s">
+        <v>38</v>
+      </c>
+      <c r="N37" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q37">
+        <f>SUM(D33,Q32)</f>
+        <v>84.15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>